<commit_message>
set for weizmann data
</commit_message>
<xml_diff>
--- a/Code/Training Code/filename_training.xlsx
+++ b/Code/Training Code/filename_training.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\TA\TugasAkhir\Code\Training Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{65EBB16D-FD9D-4A07-95D1-0B11DD222A48}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D059A745-3559-4B24-85E8-649D0814A676}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4470" activeTab="4" xr2:uid="{8BA8C306-381F-4D7C-9FEA-267794D4880B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4470" activeTab="1" xr2:uid="{8BA8C306-381F-4D7C-9FEA-267794D4880B}"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" r:id="rId1"/>
-    <sheet name="test3" sheetId="3" r:id="rId2"/>
-    <sheet name="test2" sheetId="2" r:id="rId3"/>
-    <sheet name="test4" sheetId="4" r:id="rId4"/>
-    <sheet name="pagi" sheetId="5" r:id="rId5"/>
+    <sheet name="weizmann" sheetId="1" r:id="rId1"/>
+    <sheet name="weizmann_testing" sheetId="6" r:id="rId2"/>
+    <sheet name="test3" sheetId="3" r:id="rId3"/>
+    <sheet name="test2" sheetId="2" r:id="rId4"/>
+    <sheet name="test4" sheetId="4" r:id="rId5"/>
+    <sheet name="pagi" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="167">
   <si>
     <t>daria_run.avi</t>
   </si>
@@ -202,9 +203,6 @@
     <t>ira_skip.avi</t>
   </si>
   <si>
-    <t>lena_skip2.avi</t>
-  </si>
-  <si>
     <t>lena_skip1.avi</t>
   </si>
   <si>
@@ -452,6 +450,87 @@
   </si>
   <si>
     <t>wave_pagi_zaki_4.avi</t>
+  </si>
+  <si>
+    <t>shahar_jump.avi</t>
+  </si>
+  <si>
+    <t>shahar_run.avi</t>
+  </si>
+  <si>
+    <t>shahar_walk.avi</t>
+  </si>
+  <si>
+    <t>shahar_wave2.avi</t>
+  </si>
+  <si>
+    <t>shahar_pjump.avi</t>
+  </si>
+  <si>
+    <t>shahar_jack.avi</t>
+  </si>
+  <si>
+    <t>shahar_side.avi</t>
+  </si>
+  <si>
+    <t>shahar_skip.avi</t>
+  </si>
+  <si>
+    <t>shahar_wave1.avi</t>
+  </si>
+  <si>
+    <t>lyova_jack.avi</t>
+  </si>
+  <si>
+    <t>moshe_jack.avi</t>
+  </si>
+  <si>
+    <t>lyova_side.avi</t>
+  </si>
+  <si>
+    <t>moshe_side.avi</t>
+  </si>
+  <si>
+    <t>lyova_skip.avi</t>
+  </si>
+  <si>
+    <t>moshe_skip.avi</t>
+  </si>
+  <si>
+    <t>lyova_wave1.avi</t>
+  </si>
+  <si>
+    <t>moshe_wave1.avi</t>
+  </si>
+  <si>
+    <t>lyova_run.avi</t>
+  </si>
+  <si>
+    <t>moshe_run.avi</t>
+  </si>
+  <si>
+    <t>lyova_walk.avi</t>
+  </si>
+  <si>
+    <t>moshe_walk.avi</t>
+  </si>
+  <si>
+    <t>lyova_wave2.avi</t>
+  </si>
+  <si>
+    <t>moshe_wave2.avi</t>
+  </si>
+  <si>
+    <t>lyova_jump.avi</t>
+  </si>
+  <si>
+    <t>moshe_jump.avi</t>
+  </si>
+  <si>
+    <t>lyova_pjump.avi</t>
+  </si>
+  <si>
+    <t>moshe_pjump.avi</t>
   </si>
 </sst>
 </file>
@@ -806,7 +885,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +925,7 @@
         <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -875,7 +954,7 @@
         <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -904,7 +983,7 @@
         <v>53</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -933,7 +1012,7 @@
         <v>54</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -962,7 +1041,7 @@
         <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -991,7 +1070,7 @@
         <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1017,39 +1096,39 @@
         <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1058,6 +1137,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9DD592-E606-4B47-9C4D-ABAF34A115BD}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FC9A3E-15C5-4B92-91B0-08FD8ED89A47}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1157,7 +1338,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10E9A2E-68E8-4FCB-994E-C3178F3C7489}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1206,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1217,7 +1398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C053BDC-E3EF-47F0-A7F4-5F09E808510C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1229,12 +1410,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1242,11 +1423,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01AAC3A3-FBC6-453D-9490-40617E706CD3}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -1267,237 +1448,237 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
-        <v>88</v>
-      </c>
       <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
         <v>107</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>108</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>109</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>110</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>111</v>
       </c>
-      <c r="L1" t="s">
-        <v>112</v>
-      </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
         <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>78</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>79</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>80</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>81</v>
-      </c>
-      <c r="O2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>